<commit_message>
WOrking on understanding this problem
</commit_message>
<xml_diff>
--- a/CH-035 Up and Down Grades.xlsx
+++ b/CH-035 Up and Down Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{8D358D2D-48C3-49C1-BABF-9FE493F7DC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E184C166-C9ED-4002-BA51-5784DA505488}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2298DA3E-8AB0-4836-B2A0-2E4AEBA38F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="21">
   <si>
     <t>Question</t>
   </si>
@@ -471,14 +471,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -995,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1015,20 +1015,20 @@
   <sheetData>
     <row r="1" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="34"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1320,7 +1320,7 @@
       <c r="Z7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AA7" s="32" t="s">
+      <c r="AA7" s="29" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1369,10 +1369,10 @@
       <c r="Y8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Z8" s="33" t="s">
+      <c r="Z8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="AA8" s="32" t="s">
+      <c r="AA8" s="29" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="26"/>
-      <c r="N16" s="32" t="s">
+      <c r="N16" s="29" t="s">
         <v>17</v>
       </c>
       <c r="O16">
@@ -1739,7 +1739,7 @@
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="26"/>
-      <c r="N17" s="32" t="s">
+      <c r="N17" s="29" t="s">
         <v>10</v>
       </c>
       <c r="O17">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="26"/>
-      <c r="N18" s="32" t="s">
+      <c r="N18" s="29" t="s">
         <v>12</v>
       </c>
       <c r="O18">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="26"/>
-      <c r="N19" s="32" t="s">
+      <c r="N19" s="29" t="s">
         <v>16</v>
       </c>
       <c r="O19">
@@ -1982,7 +1982,7 @@
         <v>12</v>
       </c>
       <c r="H29" s="24"/>
-      <c r="N29" s="34" t="str" cm="1">
+      <c r="N29" s="31" t="str" cm="1">
         <f t="array" ref="N29:Q33">_xlfn.LET(_xlpm.T,B2:D37,_xlpm.TT,_xlfn.DROP(_xlpm.T,1),_xlpm.M,_xlfn.TAKE(_xlpm.TT,,1),_xlpm.MM,MONTH(_xlpm.M),_xlpm.MMM,IF(_xlpm.MM=12,1,_xlpm.MM+1),_xlpm.AG,_xlfn.CHOOSECOLS(_xlpm.TT,2),_xlpm.AGU,_xlfn.UNIQUE(_xlpm.AG),_xlpm.G,_xlfn.SWITCH(_xlfn.TAKE(_xlpm.TT,,-1),"A+",1,"A",2,"B",3,"C",4),_xlpm.GCME,_xlfn.LAMBDA(_xlpm.A,_xlpm.ID,_xlfn.TAKE(_xlfn._xlws.FILTER(_xlpm.G,(_xlpm.MMM=_xlpm.A)*(_xlpm.AG=_xlpm.ID)),-1)),_xlpm.GPM,_xlfn.LAMBDA(_xlpm.A,_xlpm.ID,_xlfn.TAKE(_xlfn._xlws.FILTER(_xlpm.G,(_xlpm.MMM&lt;=_xlpm.A-1)*(_xlpm.AG=_xlpm.ID)),-1)),_xlpm.R,_xlfn.LAMBDA(_xlpm.M,_xlfn.MAP(_xlpm.AGU,_xlfn.LAMBDA(_xlpm.A,_xlpm.GCME(_xlpm.M,_xlpm.A)-_xlpm.GPM(_xlpm.M,_xlpm.A)))),_xlpm.RR,_xlfn.LAMBDA(_xlpm.B,_xlfn.CONCAT(_xlpm.B-1,SUM(--IFERROR(_xlpm.R(_xlpm.B)&lt;0,0)),SUM(--IFERROR(_xlpm.R(_xlpm.B)=0,0)),SUM(--IFERROR(_xlpm.R(_xlpm.B)&gt;0,0)))),_xlpm.NC,_xlfn.MAP(_xlfn.SEQUENCE(4,,2),_xlfn.LAMBDA(_xlpm.A,_xlpm.RR(_xlpm.A))),_xlfn.VSTACK(_xlfn.HSTACK("Month","No Upgrade","No Change","No Down-Grade"),MID(_xlpm.NC,_xlfn.SEQUENCE(,4),1)))</f>
         <v>Month</v>
       </c>
@@ -2006,7 +2006,7 @@
       <c r="D30" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="34" t="str" cm="1">
+      <c r="F30" s="31" t="str" cm="1">
         <f t="array" ref="F30:I34">_xlfn.REDUCE(_xlfn.HSTACK("Month","No "&amp;{"Upgrade","Change","Down-grade"}), {12,1,2,3}, _xlfn.LAMBDA(_xlpm.i,_xlpm.x, _xlfn.LET(_xlpm.j, MOD(_xlpm.x+1, 12), _xlpm.B, MONTH(B3:B37), _xlpm.U, _xlfn.UNIQUE(C3:C37), _xlpm.F, _xlfn.LAMBDA(_xlpm.y, _xlfn.XMATCH(_xlfn.XLOOKUP(_xlpm.y&amp;_xlpm.U, _xlpm.B&amp;C3:C37, D3:D37,,,-1), {"A+","A","B","C"})), _xlpm.M,_xlfn.TOCOL(_xlpm.F(_xlpm.j)-_xlfn.IFNA(_xlpm.F(_xlpm.x), 4), 2), _xlfn.VSTACK(_xlpm.i, _xlfn.HSTACK(_xlpm.j, SUM(N(_xlpm.M&lt;0)), SUM(N(_xlpm.M=0)), SUM(N(_xlpm.M&gt;0)))))))</f>
         <v>Month</v>
       </c>
@@ -2042,7 +2042,7 @@
       <c r="D31" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="34">
+      <c r="F31" s="31">
         <v>1</v>
       </c>
       <c r="G31">
@@ -2077,7 +2077,7 @@
       <c r="D32" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="31">
         <v>2</v>
       </c>
       <c r="G32">
@@ -2112,7 +2112,7 @@
       <c r="D33" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="34">
+      <c r="F33" s="31">
         <v>3</v>
       </c>
       <c r="G33">
@@ -2147,7 +2147,7 @@
       <c r="D34" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="34">
+      <c r="F34" s="31">
         <v>4</v>
       </c>
       <c r="G34">
@@ -2170,7 +2170,7 @@
       <c r="D35" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="H35" s="24"/>
     </row>
     <row r="36" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2183,7 +2183,7 @@
       <c r="D36" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="H36" s="24"/>
     </row>
     <row r="37" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2196,51 +2196,176 @@
       <c r="D37" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="34"/>
-      <c r="H37" s="24"/>
+      <c r="F37" s="31" t="str" cm="1">
+        <f t="array" ref="F37:I41">_xlfn.REDUCE(_xlfn.HSTACK("Month","No "&amp;{"Upgrade","Change","Down-grade"}), {12,1,2,3},
+        _xlfn.LAMBDA(_xlpm.i,_xlpm.x,
+                   _xlfn.LET( _xlpm.j, MOD(_xlpm.x+1, 12),
+                        _xlpm.B, MONTH(B3:B37),
+                        _xlpm.U, _xlfn.UNIQUE(C3:C37),
+                        _xlpm.F, _xlfn.LAMBDA(_xlpm.y, _xlfn.XMATCH(_xlfn.XLOOKUP(_xlpm.y&amp;_xlpm.U, _xlpm.B&amp;C3:C37, D3:D37,,,-1), {"A+","A","B","C"})),
+                        _xlpm.M,_xlfn.TOCOL(_xlpm.F(_xlpm.j)-_xlfn.IFNA(_xlpm.F(_xlpm.x), 4), 2),
+                        _xlfn.VSTACK(_xlpm.i,
+                               _xlfn.HSTACK(_xlpm.j,
+                                      SUM(N(_xlpm.M&lt;0)),
+                                      SUM(N(_xlpm.M=0)),
+                                      SUM(N(_xlpm.M&gt;0))
+                                     )
+                               )
+                      )
+               )
+         )</f>
+        <v>Month</v>
+      </c>
+      <c r="G37" t="str">
+        <v>No Upgrade</v>
+      </c>
+      <c r="H37" s="24" t="str">
+        <v>No Change</v>
+      </c>
+      <c r="I37" t="str">
+        <v>No Down-grade</v>
+      </c>
+      <c r="L37" cm="1">
+        <f t="array" ref="L37:L41">_xlfn.REDUCE(_xlfn.HSTACK("Month","No "&amp;{"Upgrade","Change","Down-grade"}), {12,1,2,3},
+        _xlfn.LAMBDA(_xlpm.i,_xlpm.x,
+                   _xlfn.LET(_xlpm.j, MOD(_xlpm.x+1, 12),
+                        _xlpm.B, MONTH(B3:B37),
+                        _xlpm.U, _xlfn.UNIQUE(C3:C37),
+                        _xlpm.F, _xlfn.LAMBDA(_xlpm.y, _xlfn.XMATCH(_xlfn.XLOOKUP(_xlpm.y&amp;_xlpm.U, _xlpm.B&amp;C3:C37, D3:D37,,,-1), {"A+","A","B","C"})),
+                        _xlpm.M,_xlfn.TOCOL(_xlpm.F(_xlpm.j)-_xlfn.IFNA(_xlpm.F(_xlpm.x), 4), 2),
+                        _xlfn.TOCOL(_xlpm.F(1)-_xlfn.IFNA(_xlpm.F(_xlpm.x), 4), 2)
+                       )
+               )
+         )</f>
+        <v>-3</v>
+      </c>
     </row>
     <row r="38" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="27"/>
       <c r="C38" s="28"/>
-      <c r="F38" s="34"/>
-      <c r="H38" s="24"/>
+      <c r="F38" s="31">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38" s="24">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="27"/>
       <c r="C39" s="28"/>
-      <c r="F39" s="34"/>
-      <c r="H39" s="24"/>
+      <c r="F39" s="31">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39" s="24">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="27"/>
       <c r="C40" s="28"/>
-      <c r="F40" s="34"/>
-      <c r="H40" s="24"/>
+      <c r="F40" s="31">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40" s="24">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="27"/>
       <c r="C41" s="28"/>
-      <c r="H41" s="24"/>
+      <c r="F41">
+        <v>4</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41" s="24">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>-1</v>
+      </c>
+      <c r="O41" cm="1">
+        <f t="array" ref="O41:O45">_xlfn.XMATCH(_xlfn.XLOOKUP("12"&amp;_xlfn.UNIQUE(C3:C37), MONTH(B3:B37)&amp;C3:C37, D3:D37,,,-1), {"A+","A","B","C"})</f>
+        <v>2</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="42" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
       <c r="H42" s="24"/>
+      <c r="O42">
+        <v>3</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="43" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="27"/>
       <c r="C43" s="28"/>
       <c r="H43" s="24"/>
+      <c r="O43">
+        <v>3</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="44" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
       <c r="C44" s="28"/>
       <c r="H44" s="24"/>
+      <c r="O44">
+        <v>2</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="45" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="27"/>
       <c r="C45" s="28"/>
       <c r="H45" s="24"/>
+      <c r="O45">
+        <v>4</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="46" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="27"/>
@@ -2251,88 +2376,166 @@
       <c r="B47" s="27"/>
       <c r="C47" s="28"/>
       <c r="H47" s="24"/>
+      <c r="L47" t="str" cm="1">
+        <f t="array" ref="L47:O51">_xlfn.LET(_xlpm.T,B2:D37,
+     _xlpm.TT,_xlfn.DROP(_xlpm.T,1),
+     _xlpm.M,_xlfn.TAKE(_xlpm.TT,,1),
+     _xlpm.MM,MONTH(_xlpm.M),
+     _xlpm.MMM,IF(_xlpm.MM=12,1,_xlpm.MM+1),
+     _xlpm.AG,_xlfn.CHOOSECOLS(_xlpm.TT,2),
+     _xlpm.AGU,_xlfn.UNIQUE(_xlpm.AG),
+     _xlpm.G,_xlfn.SWITCH(_xlfn.TAKE(_xlpm.TT,,-1),"A+",1,"A",2,"B",3,"C",4),
+     _xlpm.GCME,_xlfn.LAMBDA(_xlpm.A,_xlpm.ID,_xlfn.TAKE(_xlfn._xlws.FILTER(_xlpm.G,(_xlpm.MMM=_xlpm.A)*(_xlpm.AG=_xlpm.ID)),-1)),
+     _xlpm.GPM,_xlfn.LAMBDA(_xlpm.A,_xlpm.ID,_xlfn.TAKE(_xlfn._xlws.FILTER(_xlpm.G,(_xlpm.MMM&lt;=_xlpm.A-1)*(_xlpm.AG=_xlpm.ID)),-1)),
+     _xlpm.R,_xlfn.LAMBDA(_xlpm.M,_xlfn.MAP(_xlpm.AGU,_xlfn.LAMBDA(_xlpm.A,_xlpm.GCME(_xlpm.M,_xlpm.A)-_xlpm.GPM(_xlpm.M,_xlpm.A)))),
+     _xlpm.RR,_xlfn.LAMBDA(_xlpm.B,_xlfn.CONCAT(_xlpm.B-1,
+                        SUM(--IFERROR(_xlpm.R(_xlpm.B)&lt;0,0)),
+                        SUM(--IFERROR(_xlpm.R(_xlpm.B)=0,0)),
+                        SUM(--IFERROR(_xlpm.R(_xlpm.B)&gt;0,0)))),
+     _xlpm.NC,_xlfn.MAP(_xlfn.SEQUENCE(4,,2),_xlfn.LAMBDA(_xlpm.A,_xlpm.RR(_xlpm.A))),
+     _xlfn.VSTACK(_xlfn.HSTACK("Month","No Upgrade","No Change","No Down-Grade"),MID(_xlpm.NC,_xlfn.SEQUENCE(,4),1))
+    )</f>
+        <v>Month</v>
+      </c>
+      <c r="M47" t="str">
+        <v>No Upgrade</v>
+      </c>
+      <c r="N47" t="str">
+        <v>No Change</v>
+      </c>
+      <c r="O47" t="str">
+        <v>No Down-Grade</v>
+      </c>
     </row>
     <row r="48" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="27"/>
       <c r="C48" s="28"/>
       <c r="H48" s="24"/>
-    </row>
-    <row r="49" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L48" t="str">
+        <v>1</v>
+      </c>
+      <c r="M48" t="str">
+        <v>2</v>
+      </c>
+      <c r="N48" t="str">
+        <v>1</v>
+      </c>
+      <c r="O48" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="27"/>
       <c r="C49" s="28"/>
       <c r="H49" s="24"/>
-    </row>
-    <row r="50" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L49" t="str">
+        <v>2</v>
+      </c>
+      <c r="M49" t="str">
+        <v>2</v>
+      </c>
+      <c r="N49" t="str">
+        <v>1</v>
+      </c>
+      <c r="O49" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="27"/>
       <c r="C50" s="28"/>
       <c r="H50" s="24"/>
-    </row>
-    <row r="51" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L50" t="str">
+        <v>3</v>
+      </c>
+      <c r="M50" t="str">
+        <v>1</v>
+      </c>
+      <c r="N50" t="str">
+        <v>1</v>
+      </c>
+      <c r="O50" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="27"/>
       <c r="C51" s="28"/>
       <c r="H51" s="24"/>
-    </row>
-    <row r="52" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L51" t="str">
+        <v>4</v>
+      </c>
+      <c r="M51" t="str">
+        <v>4</v>
+      </c>
+      <c r="N51" t="str">
+        <v>0</v>
+      </c>
+      <c r="O51" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="27"/>
       <c r="C52" s="28"/>
       <c r="H52" s="24"/>
     </row>
-    <row r="53" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="27"/>
       <c r="C53" s="28"/>
       <c r="H53" s="24"/>
     </row>
-    <row r="54" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="27"/>
       <c r="C54" s="28"/>
       <c r="H54" s="24"/>
     </row>
-    <row r="55" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="27"/>
       <c r="C55" s="28"/>
       <c r="H55" s="24"/>
     </row>
-    <row r="56" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="27"/>
       <c r="C56" s="28"/>
       <c r="H56" s="24"/>
     </row>
-    <row r="57" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="27"/>
       <c r="C57" s="28"/>
       <c r="H57" s="24"/>
     </row>
-    <row r="58" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="27"/>
       <c r="C58" s="28"/>
       <c r="H58" s="24"/>
     </row>
-    <row r="59" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="27"/>
       <c r="C59" s="28"/>
       <c r="H59" s="24"/>
     </row>
-    <row r="60" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="27"/>
       <c r="C60" s="28"/>
       <c r="H60" s="24"/>
     </row>
-    <row r="61" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="27"/>
       <c r="C61" s="28"/>
       <c r="H61" s="24"/>
     </row>
-    <row r="62" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="27"/>
       <c r="C62" s="28"/>
       <c r="H62" s="24"/>
     </row>
-    <row r="63" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="27"/>
       <c r="C63" s="28"/>
       <c r="H63" s="24"/>
     </row>
-    <row r="64" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="27"/>
       <c r="C64" s="28"/>
       <c r="H64" s="24"/>
@@ -7023,7 +7226,7 @@
     <mergeCell ref="H1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Getting closer to figuring it out
</commit_message>
<xml_diff>
--- a/CH-035 Up and Down Grades.xlsx
+++ b/CH-035 Up and Down Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2298DA3E-8AB0-4836-B2A0-2E4AEBA38F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4494551F-690A-46B6-8250-F5903DC3C027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="21">
   <si>
     <t>Question</t>
   </si>
@@ -134,7 +134,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dddd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +178,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +208,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -405,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -479,6 +491,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1013,7 +1032,7 @@
     <col min="12" max="26" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="32" t="s">
         <v>0</v>
@@ -1055,7 +1074,7 @@
       </c>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -1107,7 +1126,7 @@
       </c>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="9">
         <v>45291</v>
@@ -1149,7 +1168,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="9">
         <v>45291</v>
@@ -1191,7 +1210,7 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="9">
         <v>45291</v>
@@ -1233,7 +1252,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="9">
         <v>45291</v>
@@ -1275,7 +1294,7 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="9">
         <v>45291</v>
@@ -1324,7 +1343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="9">
         <v>45298</v>
@@ -1376,7 +1395,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="9">
         <v>45301</v>
@@ -1412,40 +1431,50 @@
         <f t="array" ref="S9">_xlfn.LET(_xlpm.z,_xlfn._xlws.FILTER($B$3:$D$37,(MONTH($B$3:$B$37)=$N9)*($C$3:$C$37=S$7)),_xlpm.x,_xlfn.TAKE(_xlfn._xlws.FILTER($B$3:$D$37,(MONTH($B$3:$B$37)=$N9)*($C$3:$C$37=S$7)),,1),_xlpm.mx,MAX(_xlpm.x),_xlfn.XLOOKUP(IFERROR(_xlfn.XLOOKUP(_xlpm.mx,_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)),""),$N$16:$N$19,$O$16:$O$19,""))</f>
         <v>2</v>
       </c>
-      <c r="T9" s="2" cm="1">
-        <f t="array" ref="T9">_xlfn.SWITCH(TRUE,LEN(O9)=0,"",O9&gt;O8,1,O9&lt;O8,-1,O9=O8,0,"A")</f>
-        <v>1</v>
-      </c>
-      <c r="U9" s="2" cm="1">
-        <f t="array" ref="U9">_xlfn.SWITCH(TRUE,LEN(P9)=0,"",P9&gt;P8,1,P9&lt;P8,-1,P9=P8,0,"A")</f>
+      <c r="T9" s="36" cm="1">
+        <f t="array" ref="T9">_xlfn.SWITCH(TRUE,LEN(O9)=0,"",O9&gt;_xlfn.XLOOKUP(TRUE,LEN(O$8:O8)&gt;0,O$8:O8,,,-1),1,O9&lt;_xlfn.XLOOKUP(TRUE,LEN(O$8:O8)&gt;0,O$8:O8,,,-1),-1,O9=_xlfn.XLOOKUP(TRUE,LEN(O$8:O8)&gt;0,O$8:O8,,,-1),0,"A")</f>
+        <v>1</v>
+      </c>
+      <c r="U9" s="36" cm="1">
+        <f t="array" ref="U9">_xlfn.SWITCH(TRUE,LEN(P9)=0,"",P9&gt;_xlfn.XLOOKUP(TRUE,LEN(P$8:P8)&gt;0,P$8:P8,,,-1),1,P9&lt;_xlfn.XLOOKUP(TRUE,LEN(P$8:P8)&gt;0,P$8:P8,,,-1),-1,P9=_xlfn.XLOOKUP(TRUE,LEN(P$8:P8)&gt;0,P$8:P8,,,-1),0,"A")</f>
         <v>0</v>
       </c>
-      <c r="V9" s="2" cm="1">
-        <f t="array" ref="V9">_xlfn.SWITCH(TRUE,LEN(Q9)=0,"",Q9&gt;Q8,1,Q9&lt;Q8,-1,Q9=Q8,0,"A")</f>
+      <c r="V9" s="36" cm="1">
+        <f t="array" ref="V9">_xlfn.SWITCH(TRUE,LEN(Q9)=0,"",Q9&gt;_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q8)&gt;0,Q$8:Q8,,,-1),1,Q9&lt;_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q8)&gt;0,Q$8:Q8,,,-1),-1,Q9=_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q8)&gt;0,Q$8:Q8,,,-1),0,"A")</f>
         <v>-1</v>
       </c>
-      <c r="W9" s="2" cm="1">
-        <f t="array" ref="W9">_xlfn.SWITCH(TRUE,LEN(R9)=0,"",R9&gt;R8,1,R9&lt;R8,-1,R9=R8,0,"A")</f>
+      <c r="W9" s="36" cm="1">
+        <f t="array" ref="W9">_xlfn.SWITCH(TRUE,LEN(R9)=0,"",R9&gt;_xlfn.XLOOKUP(TRUE,LEN(R$8:R8)&gt;0,R$8:R8,,,-1),1,R9&lt;_xlfn.XLOOKUP(TRUE,LEN(R$8:R8)&gt;0,R$8:R8,,,-1),-1,R9=_xlfn.XLOOKUP(TRUE,LEN(R$8:R8)&gt;0,R$8:R8,,,-1),0,"A")</f>
         <v>-1</v>
       </c>
-      <c r="X9" s="2" cm="1">
-        <f t="array" ref="X9">_xlfn.SWITCH(TRUE,LEN(S9)=0,"",S9&gt;S8,1,S9&lt;S8,-1,S9=S8,0,"A")</f>
+      <c r="X9" s="36" cm="1">
+        <f t="array" ref="X9">_xlfn.SWITCH(TRUE,LEN(S9)=0,"",S9&gt;_xlfn.XLOOKUP(TRUE,LEN(S$8:S8)&gt;0,S$8:S8,,,-1),1,S9&lt;_xlfn.XLOOKUP(TRUE,LEN(S$8:S8)&gt;0,S$8:S8,,,-1),-1,S9=_xlfn.XLOOKUP(TRUE,LEN(S$8:S8)&gt;0,S$8:S8,,,-1),0,"A")</f>
         <v>1</v>
       </c>
       <c r="Y9" s="2">
-        <f>COUNTIF($T9:$X9,Y$8)</f>
+        <f t="shared" ref="Y9:AA12" si="0">COUNTIF($T9:$X9,Y$8)</f>
         <v>2</v>
       </c>
       <c r="Z9" s="2">
-        <f t="shared" ref="Z9:AA12" si="0">COUNTIF($T9:$X9,Z$8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AA9" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC9" t="b" cm="1">
+        <f t="array" ref="AC9:AE12">Y9:AA12=AD15:AF18</f>
+        <v>1</v>
+      </c>
+      <c r="AD9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="9">
         <v>45303</v>
@@ -1481,28 +1510,28 @@
         <f t="array" ref="S10">_xlfn.LET(_xlpm.z,_xlfn._xlws.FILTER($B$3:$D$37,(MONTH($B$3:$B$37)=$N10)*($C$3:$C$37=S$7)),_xlpm.x,_xlfn.TAKE(_xlfn._xlws.FILTER($B$3:$D$37,(MONTH($B$3:$B$37)=$N10)*($C$3:$C$37=S$7)),,1),_xlpm.mx,MAX(_xlpm.x),_xlfn.XLOOKUP(IFERROR(_xlfn.XLOOKUP(_xlpm.mx,_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)),""),$N$16:$N$19,$O$16:$O$19,""))</f>
         <v>3</v>
       </c>
-      <c r="T10" s="2" cm="1">
-        <f t="array" ref="T10">_xlfn.SWITCH(TRUE,LEN(O10)=0,"",O10&gt;O9,1,O10&lt;O9,-1,O10=O9,0,"A")</f>
+      <c r="T10" s="36" cm="1">
+        <f t="array" ref="T10">_xlfn.SWITCH(TRUE,LEN(O10)=0,"",O10&gt;_xlfn.XLOOKUP(TRUE,LEN(O$8:O9)&gt;0,O$8:O9,,,-1),1,O10&lt;_xlfn.XLOOKUP(TRUE,LEN(O$8:O9)&gt;0,O$8:O9,,,-1),-1,O10=_xlfn.XLOOKUP(TRUE,LEN(O$8:O9)&gt;0,O$8:O9,,,-1),0,"A")</f>
         <v>-1</v>
       </c>
-      <c r="U10" s="2" t="str" cm="1">
-        <f t="array" ref="U10">_xlfn.SWITCH(TRUE,LEN(P10)=0,"",P10&gt;P9,1,P10&lt;P9,-1,P10=P9,0,"A")</f>
+      <c r="U10" s="36" t="str" cm="1">
+        <f t="array" ref="U10">_xlfn.SWITCH(TRUE,LEN(P10)=0,"",P10&gt;_xlfn.XLOOKUP(TRUE,LEN(P$8:P9)&gt;0,P$8:P9,,,-1),1,P10&lt;_xlfn.XLOOKUP(TRUE,LEN(P$8:P9)&gt;0,P$8:P9,,,-1),-1,P10=_xlfn.XLOOKUP(TRUE,LEN(P$8:P9)&gt;0,P$8:P9,,,-1),0,"A")</f>
         <v/>
       </c>
-      <c r="V10" s="2" cm="1">
-        <f t="array" ref="V10">_xlfn.SWITCH(TRUE,LEN(Q10)=0,"",Q10&gt;Q9,1,Q10&lt;Q9,-1,Q10=Q9,0,"A")</f>
-        <v>1</v>
-      </c>
-      <c r="W10" s="2" cm="1">
-        <f t="array" ref="W10">_xlfn.SWITCH(TRUE,LEN(R10)=0,"",R10&gt;R9,1,R10&lt;R9,-1,R10=R9,0,"A")</f>
+      <c r="V10" s="36" cm="1">
+        <f t="array" ref="V10">_xlfn.SWITCH(TRUE,LEN(Q10)=0,"",Q10&gt;_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q9)&gt;0,Q$8:Q9,,,-1),1,Q10&lt;_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q9)&gt;0,Q$8:Q9,,,-1),-1,Q10=_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q9)&gt;0,Q$8:Q9,,,-1),0,"A")</f>
+        <v>1</v>
+      </c>
+      <c r="W10" s="36" cm="1">
+        <f t="array" ref="W10">_xlfn.SWITCH(TRUE,LEN(R10)=0,"",R10&gt;_xlfn.XLOOKUP(TRUE,LEN(R$8:R9)&gt;0,R$8:R9,,,-1),1,R10&lt;_xlfn.XLOOKUP(TRUE,LEN(R$8:R9)&gt;0,R$8:R9,,,-1),-1,R10=_xlfn.XLOOKUP(TRUE,LEN(R$8:R9)&gt;0,R$8:R9,,,-1),0,"A")</f>
         <v>0</v>
       </c>
-      <c r="X10" s="2" cm="1">
-        <f t="array" ref="X10">_xlfn.SWITCH(TRUE,LEN(S10)=0,"",S10&gt;S9,1,S10&lt;S9,-1,S10=S9,0,"A")</f>
+      <c r="X10" s="36" cm="1">
+        <f t="array" ref="X10">_xlfn.SWITCH(TRUE,LEN(S10)=0,"",S10&gt;_xlfn.XLOOKUP(TRUE,LEN(S$8:S9)&gt;0,S$8:S9,,,-1),1,S10&lt;_xlfn.XLOOKUP(TRUE,LEN(S$8:S9)&gt;0,S$8:S9,,,-1),-1,S10=_xlfn.XLOOKUP(TRUE,LEN(S$8:S9)&gt;0,S$8:S9,,,-1),0,"A")</f>
         <v>1</v>
       </c>
       <c r="Y10" s="2">
-        <f t="shared" ref="Y10:Y12" si="1">COUNTIF($T10:$X10,Y$8)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Z10" s="2">
@@ -1513,8 +1542,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="9">
         <v>45308</v>
@@ -1550,40 +1588,49 @@
         <f t="array" ref="S11">_xlfn.LET(_xlpm.z,_xlfn._xlws.FILTER($B$3:$D$37,(MONTH($B$3:$B$37)=$N11)*($C$3:$C$37=S$7)),_xlpm.x,_xlfn.TAKE(_xlfn._xlws.FILTER($B$3:$D$37,(MONTH($B$3:$B$37)=$N11)*($C$3:$C$37=S$7)),,1),_xlpm.mx,MAX(_xlpm.x),_xlfn.XLOOKUP(IFERROR(_xlfn.XLOOKUP(_xlpm.mx,_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)),""),$N$16:$N$19,$O$16:$O$19,""))</f>
         <v/>
       </c>
-      <c r="T11" s="2" t="str" cm="1">
-        <f t="array" ref="T11">_xlfn.SWITCH(TRUE,LEN(O11)=0,"",O11&gt;O10,1,O11&lt;O10,-1,O11=O10,0,"A")</f>
+      <c r="T11" s="36" t="str" cm="1">
+        <f t="array" ref="T11">_xlfn.SWITCH(TRUE,LEN(O11)=0,"",O11&gt;_xlfn.XLOOKUP(TRUE,LEN(O$8:O10)&gt;0,O$8:O10,,,-1),1,O11&lt;_xlfn.XLOOKUP(TRUE,LEN(O$8:O10)&gt;0,O$8:O10,,,-1),-1,O11=_xlfn.XLOOKUP(TRUE,LEN(O$8:O10)&gt;0,O$8:O10,,,-1),0,"A")</f>
         <v/>
       </c>
-      <c r="U11" s="2" cm="1">
-        <f t="array" ref="U11">_xlfn.SWITCH(TRUE,LEN(P11)=0,"",P11&gt;P10,1,P11&lt;P10,-1,P11=P10,0,"A")</f>
+      <c r="U11" s="36" cm="1">
+        <f t="array" ref="U11">_xlfn.SWITCH(TRUE,LEN(P11)=0,"",P11&gt;_xlfn.XLOOKUP(TRUE,LEN(P$8:P10)&gt;0,P$8:P10,,,-1),1,P11&lt;_xlfn.XLOOKUP(TRUE,LEN(P$8:P10)&gt;0,P$8:P10,,,-1),-1,P11=_xlfn.XLOOKUP(TRUE,LEN(P$8:P10)&gt;0,P$8:P10,,,-1),0,"A")</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="36" cm="1">
+        <f t="array" ref="V11">_xlfn.SWITCH(TRUE,LEN(Q11)=0,"",Q11&gt;_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q10)&gt;0,Q$8:Q10,,,-1),1,Q11&lt;_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q10)&gt;0,Q$8:Q10,,,-1),-1,Q11=_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q10)&gt;0,Q$8:Q10,,,-1),0,"A")</f>
         <v>-1</v>
       </c>
-      <c r="V11" s="2" cm="1">
-        <f t="array" ref="V11">_xlfn.SWITCH(TRUE,LEN(Q11)=0,"",Q11&gt;Q10,1,Q11&lt;Q10,-1,Q11=Q10,0,"A")</f>
-        <v>-1</v>
-      </c>
-      <c r="W11" s="2" cm="1">
-        <f t="array" ref="W11">_xlfn.SWITCH(TRUE,LEN(R11)=0,"",R11&gt;R10,1,R11&lt;R10,-1,R11=R10,0,"A")</f>
-        <v>1</v>
-      </c>
-      <c r="X11" s="2" t="str" cm="1">
-        <f t="array" ref="X11">_xlfn.SWITCH(TRUE,LEN(S11)=0,"",S11&gt;S10,1,S11&lt;S10,-1,S11=S10,0,"A")</f>
+      <c r="W11" s="36" cm="1">
+        <f t="array" ref="W11">_xlfn.SWITCH(TRUE,LEN(R11)=0,"",R11&gt;_xlfn.XLOOKUP(TRUE,LEN(R$8:R10)&gt;0,R$8:R10,,,-1),1,R11&lt;_xlfn.XLOOKUP(TRUE,LEN(R$8:R10)&gt;0,R$8:R10,,,-1),-1,R11=_xlfn.XLOOKUP(TRUE,LEN(R$8:R10)&gt;0,R$8:R10,,,-1),0,"A")</f>
+        <v>1</v>
+      </c>
+      <c r="X11" s="36" t="str" cm="1">
+        <f t="array" ref="X11">_xlfn.SWITCH(TRUE,LEN(S11)=0,"",S11&gt;_xlfn.XLOOKUP(TRUE,LEN(S$8:S10)&gt;0,S$8:S10,,,-1),1,S11&lt;_xlfn.XLOOKUP(TRUE,LEN(S$8:S10)&gt;0,S$8:S10,,,-1),-1,S11=_xlfn.XLOOKUP(TRUE,LEN(S$8:S10)&gt;0,S$8:S10,,,-1),0,"A")</f>
         <v/>
       </c>
       <c r="Y11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Z11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA11" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AC11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="9">
         <v>45316</v>
@@ -1619,29 +1666,29 @@
         <f t="array" ref="S12">_xlfn.LET(_xlpm.z,_xlfn._xlws.FILTER($B$3:$D$37,(MONTH($B$3:$B$37)=$N12)*($C$3:$C$37=S$7)),_xlpm.x,_xlfn.TAKE(_xlfn._xlws.FILTER($B$3:$D$37,(MONTH($B$3:$B$37)=$N12)*($C$3:$C$37=S$7)),,1),_xlpm.mx,MAX(_xlpm.x),_xlfn.XLOOKUP(IFERROR(_xlfn.XLOOKUP(_xlpm.mx,_xlfn.TAKE(_xlpm.z,,1),_xlfn.TAKE(_xlpm.z,,-1)),""),$N$16:$N$19,$O$16:$O$19,""))</f>
         <v>4</v>
       </c>
-      <c r="T12" s="2" cm="1">
-        <f t="array" ref="T12">_xlfn.SWITCH(TRUE,LEN(O12)=0,"",O12&gt;O11,1,O12&lt;O11,-1,O12=O11,0,"A")</f>
-        <v>-1</v>
-      </c>
-      <c r="U12" s="2" cm="1">
-        <f t="array" ref="U12">_xlfn.SWITCH(TRUE,LEN(P12)=0,"",P12&gt;P11,1,P12&lt;P11,-1,P12=P11,0,"A")</f>
-        <v>1</v>
-      </c>
-      <c r="V12" s="2" t="str" cm="1">
-        <f t="array" ref="V12">_xlfn.SWITCH(TRUE,LEN(Q12)=0,"",Q12&gt;Q11,1,Q12&lt;Q11,-1,Q12=Q11,0,"A")</f>
+      <c r="T12" s="36" cm="1">
+        <f t="array" ref="T12">_xlfn.SWITCH(TRUE,LEN(O12)=0,"",O12&gt;_xlfn.XLOOKUP(TRUE,LEN(O$8:O11)&gt;0,O$8:O11,,,-1),1,O12&lt;_xlfn.XLOOKUP(TRUE,LEN(O$8:O11)&gt;0,O$8:O11,,,-1),-1,O12=_xlfn.XLOOKUP(TRUE,LEN(O$8:O11)&gt;0,O$8:O11,,,-1),0,"A")</f>
+        <v>1</v>
+      </c>
+      <c r="U12" s="36" cm="1">
+        <f t="array" ref="U12">_xlfn.SWITCH(TRUE,LEN(P12)=0,"",P12&gt;_xlfn.XLOOKUP(TRUE,LEN(P$8:P11)&gt;0,P$8:P11,,,-1),1,P12&lt;_xlfn.XLOOKUP(TRUE,LEN(P$8:P11)&gt;0,P$8:P11,,,-1),-1,P12=_xlfn.XLOOKUP(TRUE,LEN(P$8:P11)&gt;0,P$8:P11,,,-1),0,"A")</f>
+        <v>1</v>
+      </c>
+      <c r="V12" s="36" t="str" cm="1">
+        <f t="array" ref="V12">_xlfn.SWITCH(TRUE,LEN(Q12)=0,"",Q12&gt;_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q11)&gt;0,Q$8:Q11,,,-1),1,Q12&lt;_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q11)&gt;0,Q$8:Q11,,,-1),-1,Q12=_xlfn.XLOOKUP(TRUE,LEN(Q$8:Q11)&gt;0,Q$8:Q11,,,-1),0,"A")</f>
         <v/>
       </c>
-      <c r="W12" s="2" cm="1">
-        <f t="array" ref="W12">_xlfn.SWITCH(TRUE,LEN(R12)=0,"",R12&gt;R11,1,R12&lt;R11,-1,R12=R11,0,"A")</f>
-        <v>1</v>
-      </c>
-      <c r="X12" s="2" cm="1">
-        <f t="array" ref="X12">_xlfn.SWITCH(TRUE,LEN(S12)=0,"",S12&gt;S11,1,S12&lt;S11,-1,S12=S11,0,"A")</f>
-        <v>-1</v>
+      <c r="W12" s="36" cm="1">
+        <f t="array" ref="W12">_xlfn.SWITCH(TRUE,LEN(R12)=0,"",R12&gt;_xlfn.XLOOKUP(TRUE,LEN(R$8:R11)&gt;0,R$8:R11,,,-1),1,R12&lt;_xlfn.XLOOKUP(TRUE,LEN(R$8:R11)&gt;0,R$8:R11,,,-1),-1,R12=_xlfn.XLOOKUP(TRUE,LEN(R$8:R11)&gt;0,R$8:R11,,,-1),0,"A")</f>
+        <v>1</v>
+      </c>
+      <c r="X12" s="36" cm="1">
+        <f t="array" ref="X12">_xlfn.SWITCH(TRUE,LEN(S12)=0,"",S12&gt;_xlfn.XLOOKUP(TRUE,LEN(S$8:S11)&gt;0,S$8:S11,,,-1),1,S12&lt;_xlfn.XLOOKUP(TRUE,LEN(S$8:S11)&gt;0,S$8:S11,,,-1),-1,S12=_xlfn.XLOOKUP(TRUE,LEN(S$8:S11)&gt;0,S$8:S11,,,-1),0,"A")</f>
+        <v>1</v>
       </c>
       <c r="Y12" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="Z12" s="2">
         <f t="shared" si="0"/>
@@ -1649,10 +1696,19 @@
       </c>
       <c r="AA12" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
         <v>45321</v>
       </c>
@@ -1665,7 +1721,7 @@
       <c r="E13" s="25"/>
       <c r="H13" s="24"/>
     </row>
-    <row r="14" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9">
         <v>45326</v>
       </c>
@@ -1677,8 +1733,21 @@
       </c>
       <c r="E14" s="25"/>
       <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y14" s="2"/>
+      <c r="AC14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF14" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="9">
         <v>45327</v>
@@ -1690,8 +1759,20 @@
         <v>16</v>
       </c>
       <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC15" s="14">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="15">
+        <v>2</v>
+      </c>
+      <c r="AE15" s="16">
+        <v>1</v>
+      </c>
+      <c r="AF15" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="9">
         <v>45328</v>
@@ -1725,8 +1806,20 @@
       <c r="X16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC16" s="14">
+        <v>2</v>
+      </c>
+      <c r="AD16" s="15">
+        <v>2</v>
+      </c>
+      <c r="AE16" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF16" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="9">
         <v>45329</v>
@@ -1758,8 +1851,20 @@
       <c r="X17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC17" s="14">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="35">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="9">
         <v>45331</v>
@@ -1789,8 +1894,20 @@
         <v>1</v>
       </c>
       <c r="X18" s="2"/>
-    </row>
-    <row r="19" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC18" s="21">
+        <v>4</v>
+      </c>
+      <c r="AD18" s="22">
+        <v>4</v>
+      </c>
+      <c r="AE18" s="22">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="9">
         <v>45336</v>
@@ -1823,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="9">
         <v>45337</v>
@@ -1838,7 +1955,7 @@
       <c r="F20" s="26"/>
       <c r="H20" s="24"/>
     </row>
-    <row r="21" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="9">
         <v>45342</v>
@@ -1853,7 +1970,7 @@
       <c r="F21" s="26"/>
       <c r="H21" s="24"/>
     </row>
-    <row r="22" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="9">
         <v>45345</v>
@@ -1868,7 +1985,7 @@
       <c r="F22" s="26"/>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="9">
         <v>45349</v>
@@ -1889,7 +2006,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9">
         <v>45350</v>
       </c>
@@ -1909,7 +2026,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
         <v>45353</v>
       </c>
@@ -1929,7 +2046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="9">
         <v>45354</v>
       </c>
@@ -1947,7 +2064,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="9">
         <v>45364</v>
       </c>
@@ -1959,7 +2076,7 @@
       </c>
       <c r="H27" s="24"/>
     </row>
-    <row r="28" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="9">
         <v>45375</v>
       </c>
@@ -1971,7 +2088,7 @@
       </c>
       <c r="H28" s="24"/>
     </row>
-    <row r="29" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="9">
         <v>45379</v>
       </c>
@@ -1996,7 +2113,7 @@
         <v>No Down-Grade</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9">
         <v>45383</v>
       </c>
@@ -2032,7 +2149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="9">
         <v>45384</v>
       </c>
@@ -2067,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>45387</v>
       </c>

</xml_diff>

<commit_message>
Finally got things close
</commit_message>
<xml_diff>
--- a/CH-035 Up and Down Grades.xlsx
+++ b/CH-035 Up and Down Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24001E74-D1BE-40EE-8424-315656563EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="528" documentId="8_{24001E74-D1BE-40EE-8424-315656563EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5145E30-6516-4FDE-8E10-AE66588874D5}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="36">
   <si>
     <t>Question</t>
   </si>
@@ -140,6 +140,39 @@
   <si>
     <t>Let's being by creating a simple example to ensure that I understand what I am dong</t>
   </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Alternative Grade Matrix</t>
+  </si>
+  <si>
+    <t>Alternative Difference Matrix</t>
+  </si>
+  <si>
+    <t>No Upgrade</t>
+  </si>
+  <si>
+    <t>No Down-Grade</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>VSTACK({"Month","Upgrade","No Upgrade","Downgrade"},HSTACK({1;2;3;4},w_1,w_2,w_3))</t>
+  </si>
 </sst>
 </file>
 
@@ -149,7 +182,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dddd"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -202,6 +235,32 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Mono"/>
       <family val="2"/>
@@ -436,11 +495,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -525,8 +585,43 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
@@ -1029,18 +1124,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF1000"/>
+  <dimension ref="A1:AF1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.09765625" customWidth="1"/>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="7.09765625" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="6" width="12.296875" customWidth="1"/>
     <col min="7" max="7" width="5.5" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
@@ -2562,7 +2657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>23</v>
       </c>
@@ -2580,7 +2675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="27"/>
       <c r="C50" s="28"/>
       <c r="H50" s="24"/>
@@ -2597,7 +2692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>24</v>
       </c>
@@ -2616,233 +2711,857 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="27"/>
       <c r="C52" s="28"/>
       <c r="H52" s="24"/>
     </row>
-    <row r="53" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="36" cm="1">
-        <f t="array" ref="B53">_xlfn.XMATCH(_xlfn.XLOOKUP("1"&amp;"AG-01",MONTH(_nDate)&amp;_nAgent,_nGrade,,,-1),{"A+","A","B","C"})</f>
-        <v>1</v>
+        <f t="array" ref="B53">_xlfn.XMATCH(_xlfn.XLOOKUP("1"&amp;"AG-01",MONTH(_nDate)&amp;_nAgent,_nGrade,,,-1),{"C","B","A","A+"})</f>
+        <v>4</v>
       </c>
       <c r="C53" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B53)</f>
-        <v>=XMATCH(XLOOKUP("1"&amp;"AG-01",MONTH(_nDate)&amp;_nAgent,_nGrade,,,-1),{"A+","A","B","C"})</v>
+        <v>=XMATCH(XLOOKUP("1"&amp;"AG-01",MONTH(_nDate)&amp;_nAgent,_nGrade,,,-1),{"C","B","A","A+"})</v>
       </c>
       <c r="H53" s="24"/>
     </row>
-    <row r="54" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="27"/>
       <c r="C54" s="28"/>
       <c r="H54" s="24"/>
     </row>
-    <row r="55" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="27"/>
       <c r="C55" s="28"/>
       <c r="H55" s="24"/>
     </row>
-    <row r="56" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="27"/>
+    <row r="56" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="40" t="s">
+        <v>26</v>
+      </c>
       <c r="C56" s="28"/>
       <c r="H56" s="24"/>
     </row>
-    <row r="57" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="27"/>
-      <c r="C57" s="28"/>
+    <row r="57" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" cm="1">
+        <f t="array" ref="B57:F61">_xlfn.DROP(_xlfn.REDUCE({0,0,0,0,0}, {12,1,2,3,4},
+        _xlfn.LAMBDA(_xlpm.i,_xlpm.x,
+                   _xlfn.LET( _xlpm.j, MOD(_xlpm.x+1, 12),
+                        _xlpm.B, MONTH(B3:B37),
+                        _xlpm.U, _xlfn.UNIQUE(C3:C37),
+                        _xlpm.F,_xlfn.LAMBDA(_xlpm.y, IFERROR(_xlfn.XMATCH(_xlfn.XLOOKUP(_xlpm.y&amp;_xlpm.U, _xlpm.B&amp;C3:C37, D3:D37,,,-1), {"C","B","A","A+"}),"")),
+                        _xlpm.M,_xlpm.F(_xlpm.x),
+                        _xlfn.VSTACK(_xlpm.i,_xlfn.TOROW(_xlpm.M))
+                      )
+               )
+         ),1)</f>
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
       <c r="H57" s="24"/>
-    </row>
-    <row r="58" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="27"/>
-      <c r="C58" s="28"/>
+      <c r="I57">
+        <v>3</v>
+      </c>
+      <c r="J57">
+        <v>2</v>
+      </c>
+      <c r="K57">
+        <v>2</v>
+      </c>
+      <c r="L57">
+        <v>3</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="O57" t="b" cm="1">
+        <f t="array" ref="O57:S61">_xlfn.ANCHORARRAY(B57)=I57:M61</f>
+        <v>1</v>
+      </c>
+      <c r="P57" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q57" t="b">
+        <v>1</v>
+      </c>
+      <c r="R57" t="b">
+        <v>1</v>
+      </c>
+      <c r="S57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
       <c r="H58" s="24"/>
-    </row>
-    <row r="59" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="27"/>
-      <c r="C59" s="28"/>
+      <c r="I58">
+        <v>4</v>
+      </c>
+      <c r="J58">
+        <v>2</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="M58">
+        <v>2</v>
+      </c>
+      <c r="O58" t="b">
+        <v>1</v>
+      </c>
+      <c r="P58" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q58" t="b">
+        <v>1</v>
+      </c>
+      <c r="R58" t="b">
+        <v>1</v>
+      </c>
+      <c r="S58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="str">
+        <v/>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
       <c r="H59" s="24"/>
-    </row>
-    <row r="60" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="27"/>
-      <c r="C60" s="28"/>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59" t="s">
+        <v>25</v>
+      </c>
+      <c r="K59">
+        <v>4</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>3</v>
+      </c>
+      <c r="O59" t="b">
+        <v>1</v>
+      </c>
+      <c r="P59" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q59" t="b">
+        <v>1</v>
+      </c>
+      <c r="R59" t="b">
+        <v>1</v>
+      </c>
+      <c r="S59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" t="str">
+        <v/>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60" t="str">
+        <v/>
+      </c>
       <c r="H60" s="24"/>
-    </row>
-    <row r="61" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="27"/>
-      <c r="C61" s="28"/>
+      <c r="I60" t="s">
+        <v>25</v>
+      </c>
+      <c r="J60">
+        <v>2</v>
+      </c>
+      <c r="K60">
+        <v>3</v>
+      </c>
+      <c r="L60">
+        <v>2</v>
+      </c>
+      <c r="M60" t="s">
+        <v>25</v>
+      </c>
+      <c r="O60" t="b">
+        <v>1</v>
+      </c>
+      <c r="P60" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q60" t="b">
+        <v>1</v>
+      </c>
+      <c r="R60" t="b">
+        <v>1</v>
+      </c>
+      <c r="S60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61" t="str">
+        <v/>
+      </c>
+      <c r="E61">
+        <v>4</v>
+      </c>
+      <c r="F61">
+        <v>4</v>
+      </c>
       <c r="H61" s="24"/>
-    </row>
-    <row r="62" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="27"/>
+      <c r="I61">
+        <v>3</v>
+      </c>
+      <c r="J61">
+        <v>4</v>
+      </c>
+      <c r="K61" t="s">
+        <v>25</v>
+      </c>
+      <c r="L61">
+        <v>4</v>
+      </c>
+      <c r="M61">
+        <v>4</v>
+      </c>
+      <c r="O61" t="b">
+        <v>1</v>
+      </c>
+      <c r="P61" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q61" t="b">
+        <v>1</v>
+      </c>
+      <c r="R61" t="b">
+        <v>1</v>
+      </c>
+      <c r="S61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="41"/>
       <c r="C62" s="28"/>
       <c r="H62" s="24"/>
     </row>
-    <row r="63" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="27"/>
       <c r="C63" s="28"/>
       <c r="H63" s="24"/>
     </row>
-    <row r="64" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="27"/>
+    <row r="64" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="40" t="s">
+        <v>27</v>
+      </c>
       <c r="C64" s="28"/>
-      <c r="H64" s="24"/>
-    </row>
-    <row r="65" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="27"/>
-      <c r="C65" s="28"/>
-      <c r="H65" s="24"/>
-    </row>
-    <row r="66" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="27"/>
-      <c r="C66" s="28"/>
-      <c r="H66" s="24"/>
-    </row>
-    <row r="67" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="27"/>
-      <c r="C67" s="28"/>
-      <c r="H67" s="24"/>
-    </row>
-    <row r="68" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="27"/>
-      <c r="C68" s="28"/>
-      <c r="H68" s="24"/>
-    </row>
-    <row r="69" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="27"/>
-      <c r="C69" s="28"/>
+    </row>
+    <row r="65" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" cm="1">
+        <f t="array" ref="B65:F69">_xlfn.DROP(_xlfn.REDUCE({0,0,0,0,0}, {12,1,2,3,4},
+        _xlfn.LAMBDA(_xlpm.i,_xlpm.x,
+                   _xlfn.LET( _xlpm.B, MONTH(B3:B37),
+                        _xlpm.U, _xlfn.UNIQUE(C3:C37),
+                        _xlpm.F,_xlfn.LAMBDA(_xlpm.y, IFERROR(_xlfn.XMATCH(_xlfn.XLOOKUP(_xlpm.y&amp;_xlpm.U, _xlpm.B&amp;C3:C37, D3:D37,,,-1), {"C","B","A","A+"}),"")),
+                        _xlpm.M,_xlpm.F(_xlpm.x),
+                        _xlfn.VSTACK(_xlpm.i,_xlfn.TOROW(_xlpm.M))
+                      )
+               )
+         ),1)</f>
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="str">
+        <v/>
+      </c>
+      <c r="D67">
+        <v>4</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" t="str">
+        <v/>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69" t="str">
+        <v/>
+      </c>
+      <c r="E69">
+        <v>4</v>
+      </c>
+      <c r="F69">
+        <v>4</v>
+      </c>
       <c r="H69" s="24"/>
     </row>
-    <row r="70" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="27"/>
+    <row r="70" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="42"/>
       <c r="C70" s="28"/>
       <c r="H70" s="24"/>
     </row>
-    <row r="71" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="27"/>
-      <c r="C71" s="28"/>
+    <row r="71" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="44"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="44"/>
       <c r="H71" s="24"/>
-    </row>
-    <row r="72" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="27"/>
-      <c r="C72" s="28"/>
-      <c r="H72" s="24"/>
-    </row>
-    <row r="73" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="27"/>
-      <c r="C73" s="28"/>
-      <c r="H73" s="24"/>
-    </row>
-    <row r="74" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="27"/>
-      <c r="C74" s="28"/>
-      <c r="H74" s="24"/>
-    </row>
-    <row r="75" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="27"/>
-      <c r="C75" s="28"/>
-      <c r="H75" s="24"/>
-    </row>
-    <row r="76" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="27"/>
-      <c r="C76" s="28"/>
+      <c r="K71" t="s">
+        <v>5</v>
+      </c>
+      <c r="L71" t="s">
+        <v>28</v>
+      </c>
+      <c r="M71" t="s">
+        <v>7</v>
+      </c>
+      <c r="N71" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q71" s="33">
+        <v>1</v>
+      </c>
+      <c r="R71" s="33">
+        <v>0</v>
+      </c>
+      <c r="S71" s="33">
+        <v>-1</v>
+      </c>
+      <c r="T71" s="33">
+        <v>-1</v>
+      </c>
+      <c r="U71" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="51" cm="1">
+        <f t="array" ref="B72:F75">IFERROR(_xlfn.LET( _xlpm.zz, _xlfn.LAMBDA(_xlpm.q, _xlfn.REDUCE({0},{2,3,4,5},
+              _xlfn.LAMBDA(_xlpm.i,_xlpm.y, _xlfn.LET(_xlpm.z,_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(B65),_xlpm.q),
+              _xlpm.d, IFERROR(INDEX(_xlpm.z,_xlpm.y)-_xlfn.XLOOKUP(TRUE,ISNUMBER(INDEX(_xlpm.z,_xlfn.SEQUENCE(_xlpm.y-1))),INDEX(_xlpm.z,_xlfn.SEQUENCE(_xlpm.y-1)),,,-1),""),
+              _xlfn.VSTACK(_xlpm.i,_xlpm.d))))),
+      _xlpm.yy, _xlfn.DROP(_xlfn.REDUCE({0;0;0;0;0},{1;2;3;4;5}, _xlfn.LAMBDA(_xlpm.a,_xlpm.i, _xlfn.HSTACK(_xlpm.a,_xlpm.zz(_xlpm.i)))),1,1),
+      SIGN(_xlpm.yy)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="C72" s="51">
+        <v>0</v>
+      </c>
+      <c r="D72" s="51">
+        <v>-1</v>
+      </c>
+      <c r="E72" s="51">
+        <v>-1</v>
+      </c>
+      <c r="F72" s="51">
+        <v>1</v>
+      </c>
+      <c r="H72" s="53" cm="1">
+        <f t="array" ref="H72">SUM(((B72:F72)&gt;0)*(LEN(B72:F72)&gt;0))</f>
+        <v>2</v>
+      </c>
+      <c r="K72" t="s">
+        <v>30</v>
+      </c>
+      <c r="L72" t="s">
+        <v>31</v>
+      </c>
+      <c r="M72" t="s">
+        <v>30</v>
+      </c>
+      <c r="N72" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q72" s="33">
+        <v>-1</v>
+      </c>
+      <c r="R72" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="S72" s="33">
+        <v>1</v>
+      </c>
+      <c r="T72" s="33">
+        <v>0</v>
+      </c>
+      <c r="U72" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="51">
+        <v>-1</v>
+      </c>
+      <c r="C73" s="51" t="str">
+        <v/>
+      </c>
+      <c r="D73" s="51">
+        <v>1</v>
+      </c>
+      <c r="E73" s="51">
+        <v>0</v>
+      </c>
+      <c r="F73" s="51">
+        <v>1</v>
+      </c>
+      <c r="H73" s="53" cm="1">
+        <f t="array" ref="H73">SUM(((B73:F73)&gt;0)*(LEN(B73:F73)&gt;0))</f>
+        <v>2</v>
+      </c>
+      <c r="K73" t="s">
+        <v>31</v>
+      </c>
+      <c r="L73" t="s">
+        <v>31</v>
+      </c>
+      <c r="M73" t="s">
+        <v>30</v>
+      </c>
+      <c r="N73" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q73" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="R73" s="33">
+        <v>0</v>
+      </c>
+      <c r="S73" s="33">
+        <v>-1</v>
+      </c>
+      <c r="T73" s="33">
+        <v>1</v>
+      </c>
+      <c r="U73" s="33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="51" t="str">
+        <v/>
+      </c>
+      <c r="C74" s="51">
+        <v>0</v>
+      </c>
+      <c r="D74" s="51">
+        <v>-1</v>
+      </c>
+      <c r="E74" s="51">
+        <v>1</v>
+      </c>
+      <c r="F74" s="51" t="str">
+        <v/>
+      </c>
+      <c r="H74" s="53" cm="1">
+        <f t="array" ref="H74">SUM(((B74:F74)&gt;0)*(LEN(B74:F74)&gt;0))</f>
+        <v>1</v>
+      </c>
+      <c r="K74" t="s">
+        <v>32</v>
+      </c>
+      <c r="L74" t="s">
+        <v>30</v>
+      </c>
+      <c r="M74" t="s">
+        <v>30</v>
+      </c>
+      <c r="N74" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q74" s="33">
+        <v>1</v>
+      </c>
+      <c r="R74" s="33">
+        <v>1</v>
+      </c>
+      <c r="S74" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="T74" s="33">
+        <v>1</v>
+      </c>
+      <c r="U74" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="52">
+        <v>1</v>
+      </c>
+      <c r="C75" s="52">
+        <v>1</v>
+      </c>
+      <c r="D75" s="51" t="str">
+        <v/>
+      </c>
+      <c r="E75" s="51">
+        <v>1</v>
+      </c>
+      <c r="F75" s="46">
+        <v>1</v>
+      </c>
+      <c r="H75" s="53" cm="1">
+        <f t="array" ref="H75">SUM(((B75:F75)&gt;0)*(LEN(B75:F75)&gt;0))</f>
+        <v>4</v>
+      </c>
+      <c r="K75" t="s">
+        <v>33</v>
+      </c>
+      <c r="L75" t="s">
+        <v>33</v>
+      </c>
+      <c r="M75" t="s">
+        <v>34</v>
+      </c>
+      <c r="N75" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H76" s="24"/>
     </row>
-    <row r="77" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="27"/>
-      <c r="C77" s="28"/>
+    <row r="77" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H77" s="24"/>
     </row>
-    <row r="78" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="27"/>
-      <c r="C78" s="28"/>
+    <row r="78" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="49" t="str" cm="1">
+        <f t="array" ref="B78:E82">_xlfn.LET(_xlpm.vv, _xlfn.LET( _xlpm.zz, _xlfn.LAMBDA(_xlpm.q, _xlfn.REDUCE({0},{2,3,4,5},
+              _xlfn.LAMBDA(_xlpm.i,_xlpm.y, _xlfn.LET(_xlpm.z,_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(B65),_xlpm.q),
+              _xlpm.d, IFERROR(INDEX(_xlpm.z,_xlpm.y)-_xlfn.XLOOKUP(TRUE,ISNUMBER(INDEX(_xlpm.z,_xlfn.SEQUENCE(_xlpm.y-1))),INDEX(_xlpm.z,_xlfn.SEQUENCE(_xlpm.y-1)),,,-1),""),
+              _xlfn.VSTACK(_xlpm.i,_xlpm.d))))),
+              _xlpm.yy, _xlfn.DROP(_xlfn.REDUCE({0;0;0;0;0},{1;2;3;4;5}, _xlfn.LAMBDA(_xlpm.a,_xlpm.i, _xlfn.HSTACK(_xlpm.a,_xlpm.zz(_xlpm.i)))),1,1),
+              _xlpm.yy),
+      _xlpm.w_1, _xlfn.BYROW(_xlpm.vv, _xlfn.LAMBDA(_xlpm.row, SUM(--(_xlfn._xlws.FILTER(_xlpm.row,LEN(_xlpm.row)&gt;0)&gt;0)))),
+      _xlpm.w_2, _xlfn.BYROW(_xlpm.vv, _xlfn.LAMBDA(_xlpm.row, SUM(--(_xlfn._xlws.FILTER(_xlpm.row,LEN(_xlpm.row)&gt;0)=0)))),
+      _xlpm.w_3, _xlfn.BYROW(_xlpm.vv, _xlfn.LAMBDA(_xlpm.row, SUM(--(_xlfn._xlws.FILTER(_xlpm.row,LEN(_xlpm.row)&gt;0)&lt;0)))),
+      _xlfn.VSTACK({"Month","Upgrade","No Upgrade","Downgrade"},_xlfn.HSTACK({1;2;3;4},_xlpm.w_1,_xlpm.w_2,_xlpm.w_3)))</f>
+        <v>Month</v>
+      </c>
+      <c r="C78" s="48" t="str">
+        <v>Upgrade</v>
+      </c>
+      <c r="D78" s="48" t="str">
+        <v>No Upgrade</v>
+      </c>
+      <c r="E78" s="48" t="str">
+        <v>Downgrade</v>
+      </c>
       <c r="H78" s="24"/>
-    </row>
-    <row r="79" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="27"/>
-      <c r="C79" s="28"/>
+      <c r="J78" s="36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="50">
+        <v>1</v>
+      </c>
+      <c r="C79" s="48">
+        <v>2</v>
+      </c>
+      <c r="D79" s="47">
+        <v>1</v>
+      </c>
+      <c r="E79" s="47">
+        <v>2</v>
+      </c>
       <c r="H79" s="24"/>
     </row>
-    <row r="80" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="27"/>
-      <c r="C80" s="28"/>
+    <row r="80" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="50">
+        <v>2</v>
+      </c>
+      <c r="C80" s="48">
+        <v>2</v>
+      </c>
+      <c r="D80" s="47">
+        <v>1</v>
+      </c>
+      <c r="E80" s="47">
+        <v>1</v>
+      </c>
       <c r="H80" s="24"/>
     </row>
-    <row r="81" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="27"/>
-      <c r="C81" s="28"/>
+    <row r="81" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="50">
+        <v>3</v>
+      </c>
+      <c r="C81" s="48">
+        <v>1</v>
+      </c>
+      <c r="D81" s="47">
+        <v>1</v>
+      </c>
+      <c r="E81" s="47">
+        <v>1</v>
+      </c>
       <c r="H81" s="24"/>
-    </row>
-    <row r="82" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="27"/>
-      <c r="C82" s="28"/>
+      <c r="J81" cm="1">
+        <f t="array" ref="J81:J84">_xlfn.LET(_xlpm.vv,_xlfn.ANCHORARRAY(B72),_xlfn.BYROW(_xlpm.vv, _xlfn.LAMBDA(_xlpm.row, SUM(--(_xlpm.row&gt;0)))))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="50">
+        <v>4</v>
+      </c>
+      <c r="C82" s="48">
+        <v>4</v>
+      </c>
+      <c r="D82" s="47">
+        <v>0</v>
+      </c>
+      <c r="E82" s="47">
+        <v>0</v>
+      </c>
       <c r="H82" s="24"/>
-    </row>
-    <row r="83" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="27"/>
-      <c r="C83" s="28"/>
+      <c r="J82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="43"/>
+      <c r="C83" s="43"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
       <c r="H83" s="24"/>
-    </row>
-    <row r="84" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="27"/>
-      <c r="C84" s="28"/>
+      <c r="J83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="43"/>
+      <c r="C84" s="43"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
       <c r="H84" s="24"/>
-    </row>
-    <row r="85" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="27"/>
       <c r="C85" s="28"/>
       <c r="H85" s="24"/>
     </row>
-    <row r="86" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="27"/>
-      <c r="C86" s="28"/>
+    <row r="86" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="46" t="str" cm="1">
+        <f t="array" ref="B86:E90">_xlfn.VSTACK({"Month","Upgrade","No Change","Downgrade"},_xlfn.HSTACK({1;2;3;4},_xlfn.BYROW(_xlfn.ANCHORARRAY(B72),_xlfn.LAMBDA(_xlpm.r,COUNTIF(_xlpm.r,"&gt;0"))),_xlfn.BYROW(_xlfn.ANCHORARRAY(B72),_xlfn.LAMBDA(_xlpm.r,COUNTIF(_xlpm.r,"=0"))),_xlfn.BYROW(_xlfn.ANCHORARRAY(B72),_xlfn.LAMBDA(_xlpm.r,COUNTIF(_xlpm.r,"&lt;0")))))</f>
+        <v>Month</v>
+      </c>
+      <c r="C86" s="46" t="str">
+        <v>Upgrade</v>
+      </c>
+      <c r="D86" s="46" t="str">
+        <v>No Change</v>
+      </c>
+      <c r="E86" s="46" t="str">
+        <v>Downgrade</v>
+      </c>
+      <c r="F86" s="45"/>
       <c r="H86" s="24"/>
     </row>
-    <row r="87" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="27"/>
-      <c r="C87" s="28"/>
+    <row r="87" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+      <c r="F87" s="45"/>
       <c r="H87" s="24"/>
     </row>
-    <row r="88" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="27"/>
-      <c r="C88" s="28"/>
+    <row r="88" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88" s="45"/>
       <c r="H88" s="24"/>
     </row>
-    <row r="89" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="27"/>
-      <c r="C89" s="28"/>
+    <row r="89" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89" s="45"/>
       <c r="H89" s="24"/>
     </row>
-    <row r="90" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="27"/>
-      <c r="C90" s="28"/>
+    <row r="90" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>4</v>
+      </c>
+      <c r="C90">
+        <v>4</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
       <c r="H90" s="24"/>
     </row>
-    <row r="91" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="27"/>
       <c r="C91" s="28"/>
       <c r="H91" s="24"/>
     </row>
-    <row r="92" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="27"/>
       <c r="C92" s="28"/>
       <c r="H92" s="24"/>
     </row>
-    <row r="93" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="27"/>
       <c r="C93" s="28"/>
       <c r="H93" s="24"/>
     </row>
-    <row r="94" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="27"/>
       <c r="C94" s="28"/>
       <c r="H94" s="24"/>
     </row>
-    <row r="95" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="27"/>
       <c r="C95" s="28"/>
       <c r="H95" s="24"/>
     </row>
-    <row r="96" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="27"/>
       <c r="C96" s="28"/>
       <c r="H96" s="24"/>
@@ -2923,47 +3642,47 @@
       <c r="H111" s="24"/>
     </row>
     <row r="112" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="28"/>
+      <c r="B112" s="27"/>
       <c r="C112" s="28"/>
       <c r="H112" s="24"/>
     </row>
     <row r="113" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="28"/>
+      <c r="B113" s="27"/>
       <c r="C113" s="28"/>
       <c r="H113" s="24"/>
     </row>
     <row r="114" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="28"/>
+      <c r="B114" s="27"/>
       <c r="C114" s="28"/>
       <c r="H114" s="24"/>
     </row>
     <row r="115" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="28"/>
+      <c r="B115" s="27"/>
       <c r="C115" s="28"/>
       <c r="H115" s="24"/>
     </row>
     <row r="116" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="28"/>
+      <c r="B116" s="27"/>
       <c r="C116" s="28"/>
       <c r="H116" s="24"/>
     </row>
     <row r="117" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="28"/>
+      <c r="B117" s="27"/>
       <c r="C117" s="28"/>
       <c r="H117" s="24"/>
     </row>
     <row r="118" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="28"/>
+      <c r="B118" s="27"/>
       <c r="C118" s="28"/>
       <c r="H118" s="24"/>
     </row>
     <row r="119" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="28"/>
+      <c r="B119" s="27"/>
       <c r="C119" s="28"/>
       <c r="H119" s="24"/>
     </row>
     <row r="120" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="28"/>
+      <c r="B120" s="27"/>
       <c r="C120" s="28"/>
       <c r="H120" s="24"/>
     </row>
@@ -7366,6 +8085,42 @@
       <c r="B1000" s="28"/>
       <c r="C1000" s="28"/>
       <c r="H1000" s="24"/>
+    </row>
+    <row r="1001" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1001" s="28"/>
+      <c r="C1001" s="28"/>
+    </row>
+    <row r="1002" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1002" s="28"/>
+      <c r="C1002" s="28"/>
+    </row>
+    <row r="1003" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1003" s="28"/>
+      <c r="C1003" s="28"/>
+    </row>
+    <row r="1004" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1004" s="28"/>
+      <c r="C1004" s="28"/>
+    </row>
+    <row r="1005" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1005" s="28"/>
+      <c r="C1005" s="28"/>
+    </row>
+    <row r="1006" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1006" s="28"/>
+      <c r="C1006" s="28"/>
+    </row>
+    <row r="1007" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1007" s="28"/>
+      <c r="C1007" s="28"/>
+    </row>
+    <row r="1008" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1008" s="28"/>
+      <c r="C1008" s="28"/>
+    </row>
+    <row r="1009" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1009" s="28"/>
+      <c r="C1009" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
A single formula. Success
</commit_message>
<xml_diff>
--- a/CH-035 Up and Down Grades.xlsx
+++ b/CH-035 Up and Down Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="528" documentId="8_{24001E74-D1BE-40EE-8424-315656563EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5145E30-6516-4FDE-8E10-AE66588874D5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2764493-5776-4A5D-BE57-927CE695EFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -580,15 +580,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -596,7 +588,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -618,6 +609,14 @@
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1126,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1146,20 +1145,20 @@
   <sheetData>
     <row r="1" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="39"/>
+      <c r="H1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="51"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -2738,7 +2737,7 @@
       <c r="H55" s="24"/>
     </row>
     <row r="56" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="40" t="s">
+      <c r="B56" s="37" t="s">
         <v>26</v>
       </c>
       <c r="C56" s="28"/>
@@ -2997,7 +2996,7 @@
       </c>
     </row>
     <row r="62" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="41"/>
+      <c r="B62" s="28"/>
       <c r="C62" s="28"/>
       <c r="H62" s="24"/>
     </row>
@@ -3007,7 +3006,7 @@
       <c r="H63" s="24"/>
     </row>
     <row r="64" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="37" t="s">
         <v>27</v>
       </c>
       <c r="C64" s="28"/>
@@ -3109,15 +3108,15 @@
       <c r="H69" s="24"/>
     </row>
     <row r="70" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="42"/>
+      <c r="B70" s="38"/>
       <c r="C70" s="28"/>
       <c r="H70" s="24"/>
     </row>
     <row r="71" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C71" s="44"/>
-      <c r="D71" s="44"/>
-      <c r="E71" s="44"/>
-      <c r="F71" s="44"/>
+      <c r="C71" s="40"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="40"/>
+      <c r="F71" s="40"/>
       <c r="H71" s="24"/>
       <c r="K71" t="s">
         <v>5</v>
@@ -3148,7 +3147,7 @@
       </c>
     </row>
     <row r="72" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="51" cm="1">
+      <c r="B72" s="46" cm="1">
         <f t="array" ref="B72:F75">IFERROR(_xlfn.LET( _xlpm.zz, _xlfn.LAMBDA(_xlpm.q, _xlfn.REDUCE({0},{2,3,4,5},
               _xlfn.LAMBDA(_xlpm.i,_xlpm.y, _xlfn.LET(_xlpm.z,_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(B65),_xlpm.q),
               _xlpm.d, IFERROR(INDEX(_xlpm.z,_xlpm.y)-_xlfn.XLOOKUP(TRUE,ISNUMBER(INDEX(_xlpm.z,_xlfn.SEQUENCE(_xlpm.y-1))),INDEX(_xlpm.z,_xlfn.SEQUENCE(_xlpm.y-1)),,,-1),""),
@@ -3157,19 +3156,19 @@
       SIGN(_xlpm.yy)),"")</f>
         <v>1</v>
       </c>
-      <c r="C72" s="51">
+      <c r="C72" s="46">
         <v>0</v>
       </c>
-      <c r="D72" s="51">
+      <c r="D72" s="46">
         <v>-1</v>
       </c>
-      <c r="E72" s="51">
+      <c r="E72" s="46">
         <v>-1</v>
       </c>
-      <c r="F72" s="51">
-        <v>1</v>
-      </c>
-      <c r="H72" s="53" cm="1">
+      <c r="F72" s="46">
+        <v>1</v>
+      </c>
+      <c r="H72" s="48" cm="1">
         <f t="array" ref="H72">SUM(((B72:F72)&gt;0)*(LEN(B72:F72)&gt;0))</f>
         <v>2</v>
       </c>
@@ -3202,22 +3201,22 @@
       </c>
     </row>
     <row r="73" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="51">
+      <c r="B73" s="46">
         <v>-1</v>
       </c>
-      <c r="C73" s="51" t="str">
+      <c r="C73" s="46" t="str">
         <v/>
       </c>
-      <c r="D73" s="51">
-        <v>1</v>
-      </c>
-      <c r="E73" s="51">
+      <c r="D73" s="46">
+        <v>1</v>
+      </c>
+      <c r="E73" s="46">
         <v>0</v>
       </c>
-      <c r="F73" s="51">
-        <v>1</v>
-      </c>
-      <c r="H73" s="53" cm="1">
+      <c r="F73" s="46">
+        <v>1</v>
+      </c>
+      <c r="H73" s="48" cm="1">
         <f t="array" ref="H73">SUM(((B73:F73)&gt;0)*(LEN(B73:F73)&gt;0))</f>
         <v>2</v>
       </c>
@@ -3250,22 +3249,22 @@
       </c>
     </row>
     <row r="74" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="51" t="str">
+      <c r="B74" s="46" t="str">
         <v/>
       </c>
-      <c r="C74" s="51">
+      <c r="C74" s="46">
         <v>0</v>
       </c>
-      <c r="D74" s="51">
+      <c r="D74" s="46">
         <v>-1</v>
       </c>
-      <c r="E74" s="51">
-        <v>1</v>
-      </c>
-      <c r="F74" s="51" t="str">
+      <c r="E74" s="46">
+        <v>1</v>
+      </c>
+      <c r="F74" s="46" t="str">
         <v/>
       </c>
-      <c r="H74" s="53" cm="1">
+      <c r="H74" s="48" cm="1">
         <f t="array" ref="H74">SUM(((B74:F74)&gt;0)*(LEN(B74:F74)&gt;0))</f>
         <v>1</v>
       </c>
@@ -3298,22 +3297,22 @@
       </c>
     </row>
     <row r="75" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="52">
-        <v>1</v>
-      </c>
-      <c r="C75" s="52">
-        <v>1</v>
-      </c>
-      <c r="D75" s="51" t="str">
+      <c r="B75" s="47">
+        <v>1</v>
+      </c>
+      <c r="C75" s="47">
+        <v>1</v>
+      </c>
+      <c r="D75" s="46" t="str">
         <v/>
       </c>
-      <c r="E75" s="51">
-        <v>1</v>
-      </c>
-      <c r="F75" s="46">
-        <v>1</v>
-      </c>
-      <c r="H75" s="53" cm="1">
+      <c r="E75" s="46">
+        <v>1</v>
+      </c>
+      <c r="F75" s="41">
+        <v>1</v>
+      </c>
+      <c r="H75" s="48" cm="1">
         <f t="array" ref="H75">SUM(((B75:F75)&gt;0)*(LEN(B75:F75)&gt;0))</f>
         <v>4</v>
       </c>
@@ -3337,8 +3336,9 @@
       <c r="H77" s="24"/>
     </row>
     <row r="78" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="49" t="str" cm="1">
-        <f t="array" ref="B78:E82">_xlfn.LET(_xlpm.vv, _xlfn.LET( _xlpm.zz, _xlfn.LAMBDA(_xlpm.q, _xlfn.REDUCE({0},{2,3,4,5},
+      <c r="B78" s="44" t="str" cm="1">
+        <f t="array" ref="B78:E82">_xlfn.LET(_xlpm.vv, _xlfn.LET(
+              _xlpm.zz, _xlfn.LAMBDA(_xlpm.q, _xlfn.REDUCE({0},{2,3,4,5},
               _xlfn.LAMBDA(_xlpm.i,_xlpm.y, _xlfn.LET(_xlpm.z,_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(B65),_xlpm.q),
               _xlpm.d, IFERROR(INDEX(_xlpm.z,_xlpm.y)-_xlfn.XLOOKUP(TRUE,ISNUMBER(INDEX(_xlpm.z,_xlfn.SEQUENCE(_xlpm.y-1))),INDEX(_xlpm.z,_xlfn.SEQUENCE(_xlpm.y-1)),,,-1),""),
               _xlfn.VSTACK(_xlpm.i,_xlpm.d))))),
@@ -3350,13 +3350,13 @@
       _xlfn.VSTACK({"Month","Upgrade","No Upgrade","Downgrade"},_xlfn.HSTACK({1;2;3;4},_xlpm.w_1,_xlpm.w_2,_xlpm.w_3)))</f>
         <v>Month</v>
       </c>
-      <c r="C78" s="48" t="str">
+      <c r="C78" s="43" t="str">
         <v>Upgrade</v>
       </c>
-      <c r="D78" s="48" t="str">
+      <c r="D78" s="43" t="str">
         <v>No Upgrade</v>
       </c>
-      <c r="E78" s="48" t="str">
+      <c r="E78" s="43" t="str">
         <v>Downgrade</v>
       </c>
       <c r="H78" s="24"/>
@@ -3365,46 +3365,46 @@
       </c>
     </row>
     <row r="79" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="50">
-        <v>1</v>
-      </c>
-      <c r="C79" s="48">
+      <c r="B79" s="45">
+        <v>1</v>
+      </c>
+      <c r="C79" s="43">
         <v>2</v>
       </c>
-      <c r="D79" s="47">
-        <v>1</v>
-      </c>
-      <c r="E79" s="47">
+      <c r="D79" s="42">
+        <v>1</v>
+      </c>
+      <c r="E79" s="42">
         <v>2</v>
       </c>
       <c r="H79" s="24"/>
     </row>
     <row r="80" spans="2:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="50">
+      <c r="B80" s="45">
         <v>2</v>
       </c>
-      <c r="C80" s="48">
+      <c r="C80" s="43">
         <v>2</v>
       </c>
-      <c r="D80" s="47">
-        <v>1</v>
-      </c>
-      <c r="E80" s="47">
+      <c r="D80" s="42">
+        <v>1</v>
+      </c>
+      <c r="E80" s="42">
         <v>1</v>
       </c>
       <c r="H80" s="24"/>
     </row>
     <row r="81" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="50">
+      <c r="B81" s="45">
         <v>3</v>
       </c>
-      <c r="C81" s="48">
-        <v>1</v>
-      </c>
-      <c r="D81" s="47">
-        <v>1</v>
-      </c>
-      <c r="E81" s="47">
+      <c r="C81" s="43">
+        <v>1</v>
+      </c>
+      <c r="D81" s="42">
+        <v>1</v>
+      </c>
+      <c r="E81" s="42">
         <v>1</v>
       </c>
       <c r="H81" s="24"/>
@@ -3414,16 +3414,16 @@
       </c>
     </row>
     <row r="82" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="50">
+      <c r="B82" s="45">
         <v>4</v>
       </c>
-      <c r="C82" s="48">
+      <c r="C82" s="43">
         <v>4</v>
       </c>
-      <c r="D82" s="47">
+      <c r="D82" s="42">
         <v>0</v>
       </c>
-      <c r="E82" s="47">
+      <c r="E82" s="42">
         <v>0</v>
       </c>
       <c r="H82" s="24"/>
@@ -3432,20 +3432,20 @@
       </c>
     </row>
     <row r="83" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="43"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="44"/>
-      <c r="E83" s="44"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="40"/>
+      <c r="E83" s="40"/>
       <c r="H83" s="24"/>
       <c r="J83">
         <v>3</v>
       </c>
     </row>
     <row r="84" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="43"/>
-      <c r="C84" s="43"/>
-      <c r="D84" s="44"/>
-      <c r="E84" s="44"/>
+      <c r="B84" s="39"/>
+      <c r="C84" s="39"/>
+      <c r="D84" s="40"/>
+      <c r="E84" s="40"/>
       <c r="H84" s="24"/>
       <c r="J84">
         <v>5</v>
@@ -3457,20 +3457,19 @@
       <c r="H85" s="24"/>
     </row>
     <row r="86" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="46" t="str" cm="1">
+      <c r="B86" s="41" t="str" cm="1">
         <f t="array" ref="B86:E90">_xlfn.VSTACK({"Month","Upgrade","No Change","Downgrade"},_xlfn.HSTACK({1;2;3;4},_xlfn.BYROW(_xlfn.ANCHORARRAY(B72),_xlfn.LAMBDA(_xlpm.r,COUNTIF(_xlpm.r,"&gt;0"))),_xlfn.BYROW(_xlfn.ANCHORARRAY(B72),_xlfn.LAMBDA(_xlpm.r,COUNTIF(_xlpm.r,"=0"))),_xlfn.BYROW(_xlfn.ANCHORARRAY(B72),_xlfn.LAMBDA(_xlpm.r,COUNTIF(_xlpm.r,"&lt;0")))))</f>
         <v>Month</v>
       </c>
-      <c r="C86" s="46" t="str">
+      <c r="C86" s="41" t="str">
         <v>Upgrade</v>
       </c>
-      <c r="D86" s="46" t="str">
+      <c r="D86" s="41" t="str">
         <v>No Change</v>
       </c>
-      <c r="E86" s="46" t="str">
+      <c r="E86" s="41" t="str">
         <v>Downgrade</v>
       </c>
-      <c r="F86" s="45"/>
       <c r="H86" s="24"/>
     </row>
     <row r="87" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3486,7 +3485,6 @@
       <c r="E87">
         <v>2</v>
       </c>
-      <c r="F87" s="45"/>
       <c r="H87" s="24"/>
     </row>
     <row r="88" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3502,7 +3500,6 @@
       <c r="E88">
         <v>1</v>
       </c>
-      <c r="F88" s="45"/>
       <c r="H88" s="24"/>
     </row>
     <row r="89" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3518,7 +3515,6 @@
       <c r="E89">
         <v>1</v>
       </c>
-      <c r="F89" s="45"/>
       <c r="H89" s="24"/>
     </row>
     <row r="90" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3557,28 +3553,99 @@
       <c r="H94" s="24"/>
     </row>
     <row r="95" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="27"/>
-      <c r="C95" s="28"/>
+      <c r="B95" s="27" t="str" cm="1">
+        <f t="array" ref="B95:E99">_xlfn.LET(_xlpm.vv, _xlfn.LET(
+         _xlpm.tt,_xlfn.DROP(_xlfn.REDUCE({0,0,0,0,0}, {12,1,2,3,4},
+                   _xlfn.LAMBDA(_xlpm.i,_xlpm.x,
+                   _xlfn.LET( _xlpm.B, MONTH(B3:B37),
+                        _xlpm.U, _xlfn.UNIQUE(C3:C37),
+                        _xlpm.F,_xlfn.LAMBDA(_xlpm.y, IFERROR(_xlfn.XMATCH(_xlfn.XLOOKUP(_xlpm.y&amp;_xlpm.U, _xlpm.B&amp;C3:C37, D3:D37,,,-1), {"C","B","A","A+"}),"")),
+                        _xlpm.M,_xlpm.F(_xlpm.x),
+                        _xlfn.VSTACK(_xlpm.i,_xlfn.TOROW(_xlpm.M))
+                      )
+               )
+               ),1),
+              _xlpm.zz, _xlfn.LAMBDA(_xlpm.q, _xlfn.REDUCE({0},{2,3,4,5},
+              _xlfn.LAMBDA(_xlpm.i,_xlpm.y, _xlfn.LET(_xlpm.z,_xlfn.CHOOSECOLS(_xlpm.tt,_xlpm.q),
+              _xlpm.d, IFERROR(INDEX(_xlpm.z,_xlpm.y)-_xlfn.XLOOKUP(TRUE,ISNUMBER(INDEX(_xlpm.z,_xlfn.SEQUENCE(_xlpm.y-1))),INDEX(_xlpm.z,_xlfn.SEQUENCE(_xlpm.y-1)),,,-1),""),
+              _xlfn.VSTACK(_xlpm.i,_xlpm.d))))),
+              _xlpm.yy, _xlfn.DROP(_xlfn.REDUCE({0;0;0;0;0},{1;2;3;4;5}, _xlfn.LAMBDA(_xlpm.a,_xlpm.i, _xlfn.HSTACK(_xlpm.a,_xlpm.zz(_xlpm.i)))),1,1),
+              _xlpm.yy),
+      _xlpm.w_1, _xlfn.BYROW(_xlpm.vv, _xlfn.LAMBDA(_xlpm.row, SUM(--(_xlfn._xlws.FILTER(_xlpm.row,LEN(_xlpm.row)&gt;0)&gt;0)))),
+      _xlpm.w_2, _xlfn.BYROW(_xlpm.vv, _xlfn.LAMBDA(_xlpm.row, SUM(--(_xlfn._xlws.FILTER(_xlpm.row,LEN(_xlpm.row)&gt;0)=0)))),
+      _xlpm.w_3, _xlfn.BYROW(_xlpm.vv, _xlfn.LAMBDA(_xlpm.row, SUM(--(_xlfn._xlws.FILTER(_xlpm.row,LEN(_xlpm.row)&gt;0)&lt;0)))),
+      _xlfn.VSTACK({"Month","Upgrade","No Upgrade","Downgrade"},_xlfn.HSTACK({1;2;3;4},_xlpm.w_1,_xlpm.w_2,_xlpm.w_3)))</f>
+        <v>Month</v>
+      </c>
+      <c r="C95" s="28" t="str">
+        <v>Upgrade</v>
+      </c>
+      <c r="D95" t="str">
+        <v>No Upgrade</v>
+      </c>
+      <c r="E95" t="str">
+        <v>Downgrade</v>
+      </c>
       <c r="H95" s="24"/>
     </row>
     <row r="96" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="27"/>
-      <c r="C96" s="28"/>
+      <c r="B96" s="52">
+        <v>1</v>
+      </c>
+      <c r="C96" s="28">
+        <v>2</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>2</v>
+      </c>
       <c r="H96" s="24"/>
     </row>
     <row r="97" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="27"/>
-      <c r="C97" s="28"/>
+      <c r="B97" s="52">
+        <v>2</v>
+      </c>
+      <c r="C97" s="28">
+        <v>2</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
       <c r="H97" s="24"/>
     </row>
     <row r="98" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="27"/>
-      <c r="C98" s="28"/>
+      <c r="B98" s="52">
+        <v>3</v>
+      </c>
+      <c r="C98" s="28">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
       <c r="H98" s="24"/>
     </row>
     <row r="99" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="27"/>
-      <c r="C99" s="28"/>
+      <c r="B99" s="52">
+        <v>4</v>
+      </c>
+      <c r="C99" s="28">
+        <v>4</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
       <c r="H99" s="24"/>
     </row>
     <row r="100" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>